<commit_message>
GDE-8272: added dataset FINASTRA_CCB_FX_JB_FX07.csv, updated TL_FXRATES_07 row with invalid Funding Desk column in TL_Data_Set_EU.xlsx, changed ${ExcelPath} to ${TL_DATASET} in TL_FXRATES_07.robot
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_EU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_EU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C69E9E0-2820-442A-8703-C350A2084D82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4251131E-7276-4011-81DA-B813D39AEEED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="941">
   <si>
     <t>rowid</t>
   </si>
@@ -2900,6 +2900,9 @@
   </si>
   <si>
     <t>FINASTRA_CCB_FX_SY_FX35.csv</t>
+  </si>
+  <si>
+    <t>JB</t>
   </si>
 </sst>
 </file>
@@ -4839,9 +4842,9 @@
   <sheetPr codeName="FXRates_Fields"/>
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5239,7 +5242,7 @@
         <v>12</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>911</v>
+        <v>940</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">

</xml_diff>